<commit_message>
[UPD] Fixing the way of obtaining the ranking
</commit_message>
<xml_diff>
--- a/results/ejercicio1.xlsx
+++ b/results/ejercicio1.xlsx
@@ -486,7 +486,7 @@
         <v>0.2903967390005001</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -512,7 +512,7 @@
         <v>0.3108609849517076</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -525,7 +525,7 @@
         <v>0.3024773645699649</v>
       </c>
       <c r="C7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">

</xml_diff>